<commit_message>
added templates, adjusted format of resources.xlsx
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\aaronwong\code\ai_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Desktop/Class Material/CS 4269/ai_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4A954F-7B27-44B6-B019-4A31A0A2233E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0401A41-3A34-3C44-A5EC-8774F9233F43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="1590" windowWidth="23025" windowHeight="15555" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Resources</t>
   </si>
@@ -81,15 +81,9 @@
     <t>R21</t>
   </si>
   <si>
-    <t>analog to farm</t>
-  </si>
-  <si>
     <t>R22</t>
   </si>
   <si>
-    <t>analog to factory</t>
-  </si>
-  <si>
     <t>R1'</t>
   </si>
   <si>
@@ -135,46 +129,127 @@
     <t>R19</t>
   </si>
   <si>
-    <t>analog to population - the amount of people in a country is only a small indicator of the country's prosperity. Some small countries are very wealthy and some are very poor. Overall, does indicate some sense of wealth for a country.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analog to metallic elements; essential for metallic alloy creation and electronic creation </t>
-  </si>
-  <si>
-    <t>analog to timber - used in all forms of construction, but not a particularly rare resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analog to available land; valued at twice the weight as water because land limits how much housing/farm/factories can be created that bring large amounts of prosperity. </t>
-  </si>
-  <si>
-    <t>analog to renewable energy; renewable energy valued at 1 - in direct correlation to renewable energy waste's weight being -1</t>
-  </si>
-  <si>
-    <t>analog to fossil fuel energy - fossil fuels create more energy than green sources, but their waste is higher to indicate penalty for using nonrenewables.</t>
-  </si>
-  <si>
-    <t>analog to water; 0.5 chosen as the baseline for which all other raw resources are weighted. Essential for life and is involved in other types of resource creation, but is not rare.</t>
-  </si>
-  <si>
-    <t>analog to animals; used for farms and food. Not particularly rare and has only a few use cases</t>
-  </si>
-  <si>
-    <t>analog to plants; used for farms and food, also produces fresh oxygen. Not particularly rare as well.</t>
-  </si>
-  <si>
-    <t>analog to metallic alloys; weighted at 2 to account for -1 alloy waste weight. Alloy + alloy waste = 2 in weight, compared to 1.5 in lost input resources</t>
-  </si>
-  <si>
-    <t>analog to housing; weighted at 15 to account for -2 housing waste weight. Input resources lost have combined weight of 12.25.</t>
-  </si>
-  <si>
-    <t>analog to electronics; weighted at 5 since 2 electronics and 1 waste is created - these total to 9 in weight compared to 8.25 of lost input resources</t>
-  </si>
-  <si>
-    <t>renewable energy waste; renewable energies' waste weighted at -1 so that there is no net loss in using renewable energies</t>
-  </si>
-  <si>
-    <t>nonrenewable energy waste, nonrenewable energy waste is weighted higher than the weight of nonrenewable energy, to discourage fossil fuel use</t>
+    <t>population</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the amount of people in a country is only a small indicator of the country's prosperity. Some small countries are very wealthy and some are very poor. Overall, does indicate some sense of wealth for a country.</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>million people</t>
+  </si>
+  <si>
+    <t>million tons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">essential for metallic alloy creation and electronic creation </t>
+  </si>
+  <si>
+    <t>metallic elements</t>
+  </si>
+  <si>
+    <t>million acres</t>
+  </si>
+  <si>
+    <t>used in all forms of construction, but not a particularly rare resource</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valued at twice the weight as water because land limits how much housing/farm/factories can be created that bring large amounts of prosperity. </t>
+  </si>
+  <si>
+    <t>million kW</t>
+  </si>
+  <si>
+    <t>billion gallons</t>
+  </si>
+  <si>
+    <t>million animals</t>
+  </si>
+  <si>
+    <t>million homes</t>
+  </si>
+  <si>
+    <t>million gadgets</t>
+  </si>
+  <si>
+    <t>thousand factories</t>
+  </si>
+  <si>
+    <t>Analog to</t>
+  </si>
+  <si>
+    <t>available land</t>
+  </si>
+  <si>
+    <t>renewable energy valued at 1 - in direct correlation to renewable energy waste's weight being -1</t>
+  </si>
+  <si>
+    <t>renewable energy</t>
+  </si>
+  <si>
+    <t>fossil fuels create more energy than green sources, but their waste is higher to indicate penalty for using nonrenewables.</t>
+  </si>
+  <si>
+    <t>fossil fuel energy</t>
+  </si>
+  <si>
+    <t>0.5 chosen as the baseline for which all other raw resources are weighted. Essential for life and is involved in other types of resource creation, but is not rare.</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>used for farms and food. Not particularly rare and has only a few use cases</t>
+  </si>
+  <si>
+    <t>animals</t>
+  </si>
+  <si>
+    <t>used for farms and food, also produces fresh oxygen. Not particularly rare as well.</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>weighted at 2 to account for -1 alloy waste weight. Alloy + alloy waste = 2 in weight, compared to 1.5 in lost input resources</t>
+  </si>
+  <si>
+    <t>metallic alloys</t>
+  </si>
+  <si>
+    <t>weighted at 15 to account for -2 housing waste weight. Input resources lost have combined weight of 12.25.</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>weighted at 5 since 2 electronics and 1 waste is created - these total to 9 in weight compared to 8.25 of lost input resources</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>factory</t>
+  </si>
+  <si>
+    <t>renewable energies' waste weighted at -1 so that there is no net loss in using renewable energies</t>
+  </si>
+  <si>
+    <t>renewable energy waste</t>
+  </si>
+  <si>
+    <t>nonrenewable energy waste is weighted higher than the weight of nonrenewable energy, to discourage fossil fuel use</t>
+  </si>
+  <si>
+    <t>nonrenewable energy waste</t>
   </si>
 </sst>
 </file>
@@ -537,15 +612,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF46A24E-FC05-49AC-9CB1-7DF7878535A1}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="160.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,10 +635,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -564,10 +652,16 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -575,10 +669,16 @@
         <v>0.75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -586,10 +686,16 @@
         <v>0.5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -597,10 +703,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -608,10 +720,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -619,10 +737,16 @@
         <v>1.5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -630,10 +754,16 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -641,10 +771,16 @@
         <v>0.5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -652,10 +788,16 @@
         <v>0.5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -663,21 +805,33 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -685,10 +839,16 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -696,106 +856,118 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>-1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>-1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>-2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>-1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>-2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>-1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>-1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1">
         <v>-1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed 2 initial_state files, fixed bug allowing trades of ourResources as other countries'
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\aaronwong\code\ai_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5476419A-DA24-4AD8-A623-F1E23DD09C24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4A954F-7B27-44B6-B019-4A31A0A2233E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="3345" windowWidth="23025" windowHeight="15555" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
+    <workbookView xWindow="6735" yWindow="1590" windowWidth="23025" windowHeight="15555" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,72 +48,36 @@
     <t>R1</t>
   </si>
   <si>
-    <t>analog to population</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>analog to metallic elements</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>analog to timber</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>analog to available land</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>analog to renewable energy</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
-    <t xml:space="preserve">analog to fossil fuel energy </t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
-    <t>analog to water</t>
-  </si>
-  <si>
     <t>R8</t>
   </si>
   <si>
-    <t>analog to animals</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
-    <t>analog to plants</t>
-  </si>
-  <si>
     <t>R18</t>
   </si>
   <si>
-    <t>analog to metallic alloys</t>
-  </si>
-  <si>
-    <t>analog to housing</t>
-  </si>
-  <si>
     <t>R20</t>
   </si>
   <si>
-    <t>analog to electronics</t>
-  </si>
-  <si>
     <t>R21</t>
   </si>
   <si>
@@ -135,15 +99,9 @@
     <t>R5'</t>
   </si>
   <si>
-    <t>renewable energy waste</t>
-  </si>
-  <si>
     <t>R6'</t>
   </si>
   <si>
-    <t>nonrenewable energy waste</t>
-  </si>
-  <si>
     <t>R18'</t>
   </si>
   <si>
@@ -175,6 +133,48 @@
   </si>
   <si>
     <t>R19</t>
+  </si>
+  <si>
+    <t>analog to population - the amount of people in a country is only a small indicator of the country's prosperity. Some small countries are very wealthy and some are very poor. Overall, does indicate some sense of wealth for a country.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analog to metallic elements; essential for metallic alloy creation and electronic creation </t>
+  </si>
+  <si>
+    <t>analog to timber - used in all forms of construction, but not a particularly rare resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analog to available land; valued at twice the weight as water because land limits how much housing/farm/factories can be created that bring large amounts of prosperity. </t>
+  </si>
+  <si>
+    <t>analog to renewable energy; renewable energy valued at 1 - in direct correlation to renewable energy waste's weight being -1</t>
+  </si>
+  <si>
+    <t>analog to fossil fuel energy - fossil fuels create more energy than green sources, but their waste is higher to indicate penalty for using nonrenewables.</t>
+  </si>
+  <si>
+    <t>analog to water; 0.5 chosen as the baseline for which all other raw resources are weighted. Essential for life and is involved in other types of resource creation, but is not rare.</t>
+  </si>
+  <si>
+    <t>analog to animals; used for farms and food. Not particularly rare and has only a few use cases</t>
+  </si>
+  <si>
+    <t>analog to plants; used for farms and food, also produces fresh oxygen. Not particularly rare as well.</t>
+  </si>
+  <si>
+    <t>analog to metallic alloys; weighted at 2 to account for -1 alloy waste weight. Alloy + alloy waste = 2 in weight, compared to 1.5 in lost input resources</t>
+  </si>
+  <si>
+    <t>analog to housing; weighted at 15 to account for -2 housing waste weight. Input resources lost have combined weight of 12.25.</t>
+  </si>
+  <si>
+    <t>analog to electronics; weighted at 5 since 2 electronics and 1 waste is created - these total to 9 in weight compared to 8.25 of lost input resources</t>
+  </si>
+  <si>
+    <t>renewable energy waste; renewable energies' waste weighted at -1 so that there is no net loss in using renewable energies</t>
+  </si>
+  <si>
+    <t>nonrenewable energy waste, nonrenewable energy waste is weighted higher than the weight of nonrenewable energy, to discourage fossil fuel use</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,238 +564,238 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>0.75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>0.5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>0.5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1">
-        <v>0.9</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>0.9</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <v>-1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2">
         <v>-1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>-1.5</v>
+        <v>-2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>-0.8</v>
+        <v>-1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
-        <v>-0.9</v>
+        <v>-2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
-        <v>-0.9</v>
+        <v>-1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1">
         <v>-1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
         <v>-1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added untradeable resources, organizational changes
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\aaronwong\code\ai_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Desktop/Class Material/CS 4269/ai_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4A954F-7B27-44B6-B019-4A31A0A2233E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0401A41-3A34-3C44-A5EC-8774F9233F43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="1590" windowWidth="23025" windowHeight="15555" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Resources</t>
   </si>
@@ -81,15 +81,9 @@
     <t>R21</t>
   </si>
   <si>
-    <t>analog to farm</t>
-  </si>
-  <si>
     <t>R22</t>
   </si>
   <si>
-    <t>analog to factory</t>
-  </si>
-  <si>
     <t>R1'</t>
   </si>
   <si>
@@ -135,46 +129,127 @@
     <t>R19</t>
   </si>
   <si>
-    <t>analog to population - the amount of people in a country is only a small indicator of the country's prosperity. Some small countries are very wealthy and some are very poor. Overall, does indicate some sense of wealth for a country.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analog to metallic elements; essential for metallic alloy creation and electronic creation </t>
-  </si>
-  <si>
-    <t>analog to timber - used in all forms of construction, but not a particularly rare resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analog to available land; valued at twice the weight as water because land limits how much housing/farm/factories can be created that bring large amounts of prosperity. </t>
-  </si>
-  <si>
-    <t>analog to renewable energy; renewable energy valued at 1 - in direct correlation to renewable energy waste's weight being -1</t>
-  </si>
-  <si>
-    <t>analog to fossil fuel energy - fossil fuels create more energy than green sources, but their waste is higher to indicate penalty for using nonrenewables.</t>
-  </si>
-  <si>
-    <t>analog to water; 0.5 chosen as the baseline for which all other raw resources are weighted. Essential for life and is involved in other types of resource creation, but is not rare.</t>
-  </si>
-  <si>
-    <t>analog to animals; used for farms and food. Not particularly rare and has only a few use cases</t>
-  </si>
-  <si>
-    <t>analog to plants; used for farms and food, also produces fresh oxygen. Not particularly rare as well.</t>
-  </si>
-  <si>
-    <t>analog to metallic alloys; weighted at 2 to account for -1 alloy waste weight. Alloy + alloy waste = 2 in weight, compared to 1.5 in lost input resources</t>
-  </si>
-  <si>
-    <t>analog to housing; weighted at 15 to account for -2 housing waste weight. Input resources lost have combined weight of 12.25.</t>
-  </si>
-  <si>
-    <t>analog to electronics; weighted at 5 since 2 electronics and 1 waste is created - these total to 9 in weight compared to 8.25 of lost input resources</t>
-  </si>
-  <si>
-    <t>renewable energy waste; renewable energies' waste weighted at -1 so that there is no net loss in using renewable energies</t>
-  </si>
-  <si>
-    <t>nonrenewable energy waste, nonrenewable energy waste is weighted higher than the weight of nonrenewable energy, to discourage fossil fuel use</t>
+    <t>population</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the amount of people in a country is only a small indicator of the country's prosperity. Some small countries are very wealthy and some are very poor. Overall, does indicate some sense of wealth for a country.</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>million people</t>
+  </si>
+  <si>
+    <t>million tons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">essential for metallic alloy creation and electronic creation </t>
+  </si>
+  <si>
+    <t>metallic elements</t>
+  </si>
+  <si>
+    <t>million acres</t>
+  </si>
+  <si>
+    <t>used in all forms of construction, but not a particularly rare resource</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valued at twice the weight as water because land limits how much housing/farm/factories can be created that bring large amounts of prosperity. </t>
+  </si>
+  <si>
+    <t>million kW</t>
+  </si>
+  <si>
+    <t>billion gallons</t>
+  </si>
+  <si>
+    <t>million animals</t>
+  </si>
+  <si>
+    <t>million homes</t>
+  </si>
+  <si>
+    <t>million gadgets</t>
+  </si>
+  <si>
+    <t>thousand factories</t>
+  </si>
+  <si>
+    <t>Analog to</t>
+  </si>
+  <si>
+    <t>available land</t>
+  </si>
+  <si>
+    <t>renewable energy valued at 1 - in direct correlation to renewable energy waste's weight being -1</t>
+  </si>
+  <si>
+    <t>renewable energy</t>
+  </si>
+  <si>
+    <t>fossil fuels create more energy than green sources, but their waste is higher to indicate penalty for using nonrenewables.</t>
+  </si>
+  <si>
+    <t>fossil fuel energy</t>
+  </si>
+  <si>
+    <t>0.5 chosen as the baseline for which all other raw resources are weighted. Essential for life and is involved in other types of resource creation, but is not rare.</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>used for farms and food. Not particularly rare and has only a few use cases</t>
+  </si>
+  <si>
+    <t>animals</t>
+  </si>
+  <si>
+    <t>used for farms and food, also produces fresh oxygen. Not particularly rare as well.</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>weighted at 2 to account for -1 alloy waste weight. Alloy + alloy waste = 2 in weight, compared to 1.5 in lost input resources</t>
+  </si>
+  <si>
+    <t>metallic alloys</t>
+  </si>
+  <si>
+    <t>weighted at 15 to account for -2 housing waste weight. Input resources lost have combined weight of 12.25.</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>weighted at 5 since 2 electronics and 1 waste is created - these total to 9 in weight compared to 8.25 of lost input resources</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>factory</t>
+  </si>
+  <si>
+    <t>renewable energies' waste weighted at -1 so that there is no net loss in using renewable energies</t>
+  </si>
+  <si>
+    <t>renewable energy waste</t>
+  </si>
+  <si>
+    <t>nonrenewable energy waste is weighted higher than the weight of nonrenewable energy, to discourage fossil fuel use</t>
+  </si>
+  <si>
+    <t>nonrenewable energy waste</t>
   </si>
 </sst>
 </file>
@@ -537,15 +612,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF46A24E-FC05-49AC-9CB1-7DF7878535A1}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="160.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,10 +635,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -564,10 +652,16 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -575,10 +669,16 @@
         <v>0.75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -586,10 +686,16 @@
         <v>0.5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -597,10 +703,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -608,10 +720,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -619,10 +737,16 @@
         <v>1.5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -630,10 +754,16 @@
         <v>0.5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -641,10 +771,16 @@
         <v>0.5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -652,10 +788,16 @@
         <v>0.5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -663,21 +805,33 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -685,10 +839,16 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -696,106 +856,118 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>-1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>-1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>-2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>-1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>-2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>-1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>-1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1">
         <v>-1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created wrapper and demo
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Desktop/Class Material/CS 4269/ai_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexw/Desktop/ai_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0401A41-3A34-3C44-A5EC-8774F9233F43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80B228C-C9FC-704A-86C0-37FA283960E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
+    <workbookView xWindow="13440" yWindow="1140" windowWidth="28800" windowHeight="16640" xr2:uid="{8A4E5DEA-FA9D-43A0-A807-EAE10F7C10B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>Resources</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>nonrenewable energy waste</t>
+  </si>
+  <si>
+    <t>cash</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF46A24E-FC05-49AC-9CB1-7DF7878535A1}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -970,6 +973,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>